<commit_message>
prop paths changed in FromExcelToTXT project
</commit_message>
<xml_diff>
--- a/XStoreInstallation/Prerequisites/UserProp.xlsx
+++ b/XStoreInstallation/Prerequisites/UserProp.xlsx
@@ -197,13 +197,13 @@
     <t>storebackup.host=</t>
   </si>
   <si>
-    <t>KA23705R01</t>
-  </si>
-  <si>
-    <t>10.53.85.133</t>
-  </si>
-  <si>
-    <t>KA23705R02</t>
+    <t>xx.xx.xxx.xxx</t>
+  </si>
+  <si>
+    <t>KA63502R01</t>
+  </si>
+  <si>
+    <t>KA63502R02</t>
   </si>
   <si>
     <t>nonlead</t>
@@ -655,7 +655,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
@@ -669,7 +669,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -683,7 +683,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2">
-        <v>23705</v>
+        <v>63502</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
@@ -697,7 +697,7 @@
         <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -749,7 +749,7 @@
       </c>
       <c r="B3" s="2">
         <f>Sheet1!B6</f>
-        <v>23705</v>
+        <v>63502</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>13</v>
@@ -761,7 +761,7 @@
       </c>
       <c r="B4" s="2">
         <f>Sheet1!B4</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>14</v>
@@ -773,7 +773,7 @@
       </c>
       <c r="B5" s="6" t="str">
         <f>Sheet1!B5</f>
-        <v>KA23705R01</v>
+        <v>KA63502R01</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>15</v>
@@ -785,7 +785,7 @@
       </c>
       <c r="B6" s="6" t="str">
         <f>Sheet1!B9</f>
-        <v>KA23705R02</v>
+        <v>KA63502R02</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>16</v>

</xml_diff>